<commit_message>
IMU code added and restructured directories
</commit_message>
<xml_diff>
--- a/iPad/measurements.xlsx
+++ b/iPad/measurements.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnnyvenom/Documents/Projects/Noisebox-2018/iPad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C78AAB8-B9B0-7D47-9872-116391BDADA1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE3F9EA-CACE-0C4F-A5A6-35331BB4339A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20560" xr2:uid="{4A421AC4-F8B8-4344-8F14-5477F6E648DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="40">
   <si>
     <t>octave</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>button</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
@@ -504,7 +510,7 @@
   <dimension ref="A1:M81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1631,6 +1637,9 @@
       <c r="H41">
         <v>0</v>
       </c>
+      <c r="I41" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
@@ -1655,6 +1664,9 @@
       <c r="H42">
         <v>1</v>
       </c>
+      <c r="I42" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
@@ -1676,6 +1688,9 @@
       <c r="H43">
         <v>2</v>
       </c>
+      <c r="I43" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
@@ -1697,6 +1712,9 @@
       <c r="H44">
         <v>3</v>
       </c>
+      <c r="I44" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
@@ -1718,6 +1736,9 @@
       <c r="H45">
         <v>4</v>
       </c>
+      <c r="I45" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
@@ -1739,6 +1760,9 @@
       <c r="H46">
         <v>5</v>
       </c>
+      <c r="I46" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
@@ -1759,6 +1783,9 @@
       </c>
       <c r="H47">
         <v>6</v>
+      </c>
+      <c r="I47" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>